<commit_message>
vault backup: 2025-12-10 16:13:15
</commit_message>
<xml_diff>
--- a/projects/Capital/Bearing Temperature Monitoring/Bearing Temp Monitoring Capital Estimate.xlsx
+++ b/projects/Capital/Bearing Temperature Monitoring/Bearing Temp Monitoring Capital Estimate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10064957\My Drive\GDVault\MarthaVault\00_Inbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10064957\My Drive\GDVault\MarthaVault\projects\Capital\Bearing Temperature Monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4944EDDD-4873-406D-8D59-F12E915546CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEAE297-96A9-4405-BECC-832F94B24F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{26256806-646B-410B-99AC-2ABEBF893D43}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{26256806-646B-410B-99AC-2ABEBF893D43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,12 +114,61 @@
         </r>
       </text>
     </comment>
+    <comment ref="H56" authorId="0" shapeId="0" xr:uid="{A3B5D1FC-5D8C-4E0D-8100-0D5E83723896}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gregory Karsten:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Maximum LOS for BT = 700m</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H74" authorId="0" shapeId="0" xr:uid="{E472486B-05B8-4F35-B567-B805D16C7C5B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gregory Karsten:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1 per belt
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="89">
   <si>
     <t>Glue</t>
   </si>
@@ -344,6 +393,48 @@
   </si>
   <si>
     <t>LS02 conveyor</t>
+  </si>
+  <si>
+    <t>Gloria UG</t>
+  </si>
+  <si>
+    <t>N3 UG</t>
+  </si>
+  <si>
+    <t>Surface Plant</t>
+  </si>
+  <si>
+    <t>CV25 – 10 bearings</t>
+  </si>
+  <si>
+    <t>CV30 – 10 bearings</t>
+  </si>
+  <si>
+    <t>CV40 – 10 bearings</t>
+  </si>
+  <si>
+    <t>CV74 – 10 bearings</t>
+  </si>
+  <si>
+    <t>CV79 – 10 bearings</t>
+  </si>
+  <si>
+    <t>CV83 – 10 bearings</t>
+  </si>
+  <si>
+    <t>Cv85 – 10 bearings</t>
+  </si>
+  <si>
+    <t>CV90 – 10 bearings</t>
+  </si>
+  <si>
+    <t>Gloria sample tower conveyor 4 bearings</t>
+  </si>
+  <si>
+    <t>Seam 1 &amp; Seam 2</t>
+  </si>
+  <si>
+    <t>Surface Plant Total</t>
   </si>
 </sst>
 </file>
@@ -353,7 +444,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$R-1C09]* #,##0_-;\-[$R-1C09]* #,##0_-;_-[$R-1C09]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,6 +488,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -424,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -439,6 +544,15 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1031,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978F4542-314C-4B68-BEB6-A1F300014BA4}">
-  <dimension ref="B1:P53"/>
+  <dimension ref="B1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="S51" sqref="S51"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="P83" sqref="P83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,7 +1159,7 @@
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" customWidth="1"/>
     <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.85546875" customWidth="1"/>
     <col min="16" max="16" width="19" bestFit="1" customWidth="1"/>
@@ -1966,7 +2080,7 @@
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>21</v>
@@ -2086,7 +2200,7 @@
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>21</v>
@@ -2354,12 +2468,12 @@
         <v>949181</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>23</v>
       </c>
@@ -2367,14 +2481,595 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N56" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P56" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B57" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B58" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F58">
+        <v>5</v>
+      </c>
+      <c r="G58">
+        <v>10</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58" s="4">
+        <f>+G58*Sheet1!$E$2</f>
+        <v>75270</v>
+      </c>
+      <c r="J58" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G58</f>
+        <v>4150</v>
+      </c>
+      <c r="K58" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G58</f>
+        <v>5702.5</v>
+      </c>
+      <c r="L58" s="4">
+        <f>+Sheet1!$E$4*H58</f>
+        <v>20480</v>
+      </c>
+      <c r="M58">
+        <v>2</v>
+      </c>
+      <c r="N58" s="4">
+        <f>+M58*Sheet1!$C$13</f>
+        <v>26600</v>
+      </c>
+      <c r="O58" s="4">
+        <f>+M58*Sheet1!$C$12</f>
+        <v>4400</v>
+      </c>
+      <c r="P58" s="4">
+        <f>+N58+L58+K58+J58+I58</f>
+        <v>132202.5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B59" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F59">
+        <v>5</v>
+      </c>
+      <c r="G59">
+        <v>10</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59" s="4">
+        <f>+G59*Sheet1!$E$2</f>
+        <v>75270</v>
+      </c>
+      <c r="J59" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G59</f>
+        <v>4150</v>
+      </c>
+      <c r="K59" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G59</f>
+        <v>5702.5</v>
+      </c>
+      <c r="L59" s="4">
+        <f>+Sheet1!$E$4*H59</f>
+        <v>20480</v>
+      </c>
+      <c r="M59">
+        <v>2</v>
+      </c>
+      <c r="N59" s="4">
+        <f>+M59*Sheet1!$C$13</f>
+        <v>26600</v>
+      </c>
+      <c r="O59" s="4">
+        <f>+M59*Sheet1!$C$12</f>
+        <v>4400</v>
+      </c>
+      <c r="P59" s="4">
+        <f t="shared" ref="P59:P66" si="3">+N59+L59+K59+J59+I59</f>
+        <v>132202.5</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B60" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F60">
+        <v>5</v>
+      </c>
+      <c r="G60">
+        <v>10</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60" s="4">
+        <f>+G60*Sheet1!$E$2</f>
+        <v>75270</v>
+      </c>
+      <c r="J60" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G60</f>
+        <v>4150</v>
+      </c>
+      <c r="K60" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G60</f>
+        <v>5702.5</v>
+      </c>
+      <c r="L60" s="4">
+        <f>+Sheet1!$E$4*H60</f>
+        <v>20480</v>
+      </c>
+      <c r="M60">
+        <v>2</v>
+      </c>
+      <c r="N60" s="4">
+        <f>+M60*Sheet1!$C$13</f>
+        <v>26600</v>
+      </c>
+      <c r="O60" s="4">
+        <f>+M60*Sheet1!$C$12</f>
+        <v>4400</v>
+      </c>
+      <c r="P60" s="4">
+        <f t="shared" si="3"/>
+        <v>132202.5</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B61" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F61">
+        <v>5</v>
+      </c>
+      <c r="G61">
+        <v>10</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61" s="4">
+        <f>+G61*Sheet1!$E$2</f>
+        <v>75270</v>
+      </c>
+      <c r="J61" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G61</f>
+        <v>4150</v>
+      </c>
+      <c r="K61" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G61</f>
+        <v>5702.5</v>
+      </c>
+      <c r="L61" s="4">
+        <f>+Sheet1!$E$4*H61</f>
+        <v>20480</v>
+      </c>
+      <c r="M61">
+        <v>2</v>
+      </c>
+      <c r="N61" s="4">
+        <f>+M61*Sheet1!$C$13</f>
+        <v>26600</v>
+      </c>
+      <c r="O61" s="4">
+        <f>+M61*Sheet1!$C$12</f>
+        <v>4400</v>
+      </c>
+      <c r="P61" s="4">
+        <f t="shared" si="3"/>
+        <v>132202.5</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B62" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F62">
+        <v>5</v>
+      </c>
+      <c r="G62">
+        <v>10</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62" s="4">
+        <f>+G62*Sheet1!$E$2</f>
+        <v>75270</v>
+      </c>
+      <c r="J62" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G62</f>
+        <v>4150</v>
+      </c>
+      <c r="K62" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G62</f>
+        <v>5702.5</v>
+      </c>
+      <c r="L62" s="4">
+        <f>+Sheet1!$E$4*H62</f>
+        <v>20480</v>
+      </c>
+      <c r="M62">
+        <v>2</v>
+      </c>
+      <c r="N62" s="4">
+        <f>+M62*Sheet1!$C$13</f>
+        <v>26600</v>
+      </c>
+      <c r="O62" s="4">
+        <f>+M62*Sheet1!$C$12</f>
+        <v>4400</v>
+      </c>
+      <c r="P62" s="4">
+        <f t="shared" si="3"/>
+        <v>132202.5</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B63" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F63">
+        <v>5</v>
+      </c>
+      <c r="G63">
+        <v>10</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63" s="4">
+        <f>+G63*Sheet1!$E$2</f>
+        <v>75270</v>
+      </c>
+      <c r="J63" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G63</f>
+        <v>4150</v>
+      </c>
+      <c r="K63" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G63</f>
+        <v>5702.5</v>
+      </c>
+      <c r="L63" s="4">
+        <f>+Sheet1!$E$4*H63</f>
+        <v>20480</v>
+      </c>
+      <c r="M63">
+        <v>2</v>
+      </c>
+      <c r="N63" s="4">
+        <f>+M63*Sheet1!$C$13</f>
+        <v>26600</v>
+      </c>
+      <c r="O63" s="4">
+        <f>+M63*Sheet1!$C$12</f>
+        <v>4400</v>
+      </c>
+      <c r="P63" s="4">
+        <f t="shared" si="3"/>
+        <v>132202.5</v>
+      </c>
+    </row>
+    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B64" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F64">
+        <v>5</v>
+      </c>
+      <c r="G64">
+        <v>10</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64" s="4">
+        <f>+G64*Sheet1!$E$2</f>
+        <v>75270</v>
+      </c>
+      <c r="J64" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G64</f>
+        <v>4150</v>
+      </c>
+      <c r="K64" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G64</f>
+        <v>5702.5</v>
+      </c>
+      <c r="L64" s="4">
+        <f>+Sheet1!$E$4*H64</f>
+        <v>20480</v>
+      </c>
+      <c r="M64">
+        <v>2</v>
+      </c>
+      <c r="N64" s="4">
+        <f>+M64*Sheet1!$C$13</f>
+        <v>26600</v>
+      </c>
+      <c r="O64" s="4">
+        <f>+M64*Sheet1!$C$12</f>
+        <v>4400</v>
+      </c>
+      <c r="P64" s="4">
+        <f t="shared" si="3"/>
+        <v>132202.5</v>
+      </c>
+    </row>
+    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B65" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F65">
+        <v>5</v>
+      </c>
+      <c r="G65">
+        <v>10</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65" s="4">
+        <f>+G65*Sheet1!$E$2</f>
+        <v>75270</v>
+      </c>
+      <c r="J65" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G65</f>
+        <v>4150</v>
+      </c>
+      <c r="K65" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G65</f>
+        <v>5702.5</v>
+      </c>
+      <c r="L65" s="4">
+        <f>+Sheet1!$E$4*H65</f>
+        <v>20480</v>
+      </c>
+      <c r="M65">
+        <v>2</v>
+      </c>
+      <c r="N65" s="4">
+        <f>+M65*Sheet1!$C$13</f>
+        <v>26600</v>
+      </c>
+      <c r="O65" s="4">
+        <f>+M65*Sheet1!$C$12</f>
+        <v>4400</v>
+      </c>
+      <c r="P65" s="4">
+        <f t="shared" si="3"/>
+        <v>132202.5</v>
+      </c>
+    </row>
+    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B66" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
+      </c>
+      <c r="G66">
+        <v>4</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66" s="4">
+        <f>+G66*Sheet1!$E$2</f>
+        <v>30108</v>
+      </c>
+      <c r="J66" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G66</f>
+        <v>1660</v>
+      </c>
+      <c r="K66" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G66</f>
+        <v>2281</v>
+      </c>
+      <c r="L66" s="4">
+        <f>+Sheet1!$E$4*H66</f>
+        <v>20480</v>
+      </c>
+      <c r="M66">
+        <v>2</v>
+      </c>
+      <c r="N66" s="4">
+        <f>+M66*Sheet1!$C$13</f>
+        <v>26600</v>
+      </c>
+      <c r="O66" s="4">
+        <f>+M66*Sheet1!$C$12</f>
+        <v>4400</v>
+      </c>
+      <c r="P66" s="4">
+        <f t="shared" si="3"/>
+        <v>81129</v>
+      </c>
+    </row>
+    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P67" s="5">
+        <f>SUM(P58:P66)</f>
+        <v>1138749</v>
+      </c>
+    </row>
+    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N68" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="O68" s="6"/>
+    </row>
+    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N69" t="s">
+        <v>7</v>
+      </c>
+      <c r="P69" s="4">
+        <f>+Sheet1!$C$11*2</f>
+        <v>33024</v>
+      </c>
+    </row>
+    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N70" t="s">
+        <v>43</v>
+      </c>
+      <c r="P70" s="4">
+        <f>+Sheet1!$C$10*2</f>
+        <v>19200</v>
+      </c>
+    </row>
+    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N71" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="O71" s="8"/>
+      <c r="P71" s="9">
+        <f>+P70+P69+P66+P63+P64+P65+P62+P61+P60+P59+P58</f>
+        <v>1190973</v>
+      </c>
+    </row>
+    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B74" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F74">
+        <f>+G74/2</f>
+        <v>178</v>
+      </c>
+      <c r="G74">
+        <v>356</v>
+      </c>
+      <c r="H74">
+        <v>39</v>
+      </c>
+      <c r="I74" s="4">
+        <f>+G74*Sheet1!$E$2</f>
+        <v>2679612</v>
+      </c>
+      <c r="J74" s="4">
+        <f>+(Sheet1!$E$5+Sheet1!$E$6)*G74</f>
+        <v>147740</v>
+      </c>
+      <c r="K74" s="4">
+        <f>+(Sheet1!$E$7+Sheet1!$E$8)*G74</f>
+        <v>203009</v>
+      </c>
+      <c r="L74" s="4">
+        <f>+Sheet1!$E$4*H74</f>
+        <v>798720</v>
+      </c>
+      <c r="M74">
+        <v>90</v>
+      </c>
+      <c r="N74" s="4">
+        <f>+M74*Sheet1!$C$13</f>
+        <v>1197000</v>
+      </c>
+      <c r="O74" s="4">
+        <f>+M74*Sheet1!$C$12</f>
+        <v>198000</v>
+      </c>
+      <c r="P74" s="5">
+        <f t="shared" ref="P74" si="4">+N74+L74+K74+J74+I74</f>
+        <v>5026081</v>
+      </c>
+    </row>
+    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N76" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="O76" s="6"/>
+    </row>
+    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N77" t="s">
+        <v>7</v>
+      </c>
+      <c r="P77" s="4">
+        <f>+Sheet1!$C$11*2</f>
+        <v>33024</v>
+      </c>
+    </row>
+    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N78" t="s">
+        <v>43</v>
+      </c>
+      <c r="P78" s="4">
+        <f>+Sheet1!$C$10*2</f>
+        <v>19200</v>
+      </c>
+    </row>
+    <row r="79" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N79" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="O79" s="8"/>
+      <c r="P79" s="9">
+        <f>+P78+P77+P74</f>
+        <v>5078305</v>
+      </c>
+    </row>
+    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B81" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N81" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="O81" s="8"/>
+      <c r="P81" s="9">
+        <f>+P79+P71</f>
+        <v>6269278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2025-12-11 14:10:54
</commit_message>
<xml_diff>
--- a/projects/Capital/Bearing Temperature Monitoring/Bearing Temp Monitoring Capital Estimate.xlsx
+++ b/projects/Capital/Bearing Temperature Monitoring/Bearing Temp Monitoring Capital Estimate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10064957\My Drive\GDVault\MarthaVault\projects\Capital\Bearing Temperature Monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEAE297-96A9-4405-BECC-832F94B24F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45602891-2200-4E8F-A316-DC5F8C408BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{26256806-646B-410B-99AC-2ABEBF893D43}"/>
   </bookViews>
@@ -1145,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978F4542-314C-4B68-BEB6-A1F300014BA4}">
-  <dimension ref="B1:P81"/>
+  <dimension ref="B1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="P83" sqref="P83"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="R75" sqref="R75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3072,6 +3072,12 @@
         <v>6269278</v>
       </c>
     </row>
+    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P85" s="4">
+        <f>+P81+P45+P33+P25+3000000</f>
+        <v>15892209</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>